<commit_message>
Refactor GaussianFilter to use an independent output buffer. Add a StopWatch class.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Array Fill</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Questions</t>
-  </si>
-  <si>
-    <t>Why is this not much slower than NOOP?</t>
   </si>
   <si>
     <t>gaussian_filter(a, sigma, order=0, …)</t>
@@ -138,6 +135,12 @@
       </rPr>
       <t xml:space="preserve"> there is no performance difference.</t>
     </r>
+  </si>
+  <si>
+    <t>full implementation (+ GetOffsetImageElement)</t>
+  </si>
+  <si>
+    <t>512 Depth Buffer</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J16"/>
+  <dimension ref="B5:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,21 +547,24 @@
     <col min="12" max="12" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>1.2E-2</v>
       </c>
@@ -578,13 +584,23 @@
       <c r="H7" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>6.0659999999999998</v>
+      </c>
+      <c r="M7">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <f>L7/M7</f>
+        <v>551.4545454545455</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>2048</v>
@@ -597,7 +613,7 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -609,9 +625,9 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>1.6E-2</v>
@@ -622,12 +638,12 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13">
@@ -639,14 +655,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -666,39 +682,48 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
-        <v>0.309</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15">
         <v>2048</v>
       </c>
       <c r="F15">
-        <v>12.195</v>
+        <v>11.948</v>
       </c>
       <c r="H15" s="5">
         <f>F15/$B$15</f>
-        <v>39.466019417475728</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+        <v>44.749063670411985</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="9"/>
       <c r="F16">
-        <v>12.222</v>
+        <v>19.204000000000001</v>
       </c>
       <c r="H16" s="5">
         <f>F16/$B$15</f>
-        <v>39.553398058252426</v>
-      </c>
-      <c r="J16" t="s">
-        <v>12</v>
+        <v>71.925093632958806</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>103.04900000000001</v>
+      </c>
+      <c r="H17" s="5">
+        <f>F17/$B$15</f>
+        <v>385.95131086142322</v>
       </c>
     </row>
   </sheetData>
@@ -723,17 +748,17 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement GaussianBlur1A which pre-computes the kernel.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Array Fill</t>
   </si>
@@ -140,7 +141,16 @@
     <t>full implementation (+ GetOffsetImageElement)</t>
   </si>
   <si>
-    <t>512 Depth Buffer</t>
+    <t>GaussianBlur1</t>
+  </si>
+  <si>
+    <t>GaussianBlur1Prime</t>
+  </si>
+  <si>
+    <t>benchmark (2048, 2048)</t>
+  </si>
+  <si>
+    <t>Explorer (512, 512)</t>
   </si>
 </sst>
 </file>
@@ -212,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -242,6 +252,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:N17"/>
+  <dimension ref="B5:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,24 +560,21 @@
     <col min="12" max="12" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>1.2E-2</v>
       </c>
@@ -584,18 +594,8 @@
       <c r="H7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L7">
-        <v>6.0659999999999998</v>
-      </c>
-      <c r="M7">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="N7">
-        <f>L7/M7</f>
-        <v>551.4545454545455</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
@@ -613,7 +613,7 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -638,7 +638,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
@@ -655,12 +655,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -682,48 +682,95 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <v>0.26700000000000002</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15">
+      <c r="D17" s="9"/>
+      <c r="E17">
         <v>2048</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>11.948</v>
       </c>
-      <c r="H15" s="5">
-        <f>F15/$B$15</f>
+      <c r="H17" s="5">
+        <f>F17/$B$17</f>
         <v>44.749063670411985</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="F16">
+      <c r="D18" s="9"/>
+      <c r="F18">
         <v>19.204000000000001</v>
       </c>
-      <c r="H16" s="5">
-        <f>F16/$B$15</f>
+      <c r="H18" s="5">
+        <f>F18/$B$17</f>
         <v>71.925093632958806</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>103.04900000000001</v>
       </c>
-      <c r="H17" s="5">
-        <f>F17/$B$15</f>
+      <c r="H19" s="5">
+        <f>F19/$B$17</f>
         <v>385.95131086142322</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21">
+        <v>10.555999999999999</v>
+      </c>
+      <c r="H21" s="5">
+        <f>F21/$B$21</f>
+        <v>959.63636363636363</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>7.0979999999999999</v>
+      </c>
+      <c r="H22" s="5">
+        <f>F22/$B$21</f>
+        <v>645.27272727272725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor GaussianKernel to dynamically allocate kernel size based on sigma.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -157,6 +157,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -270,7 +273,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -308,10 +310,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,9 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
-    </sheetView>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -613,14 +616,14 @@
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="24" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" style="4" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="24" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
     <col min="15" max="15" width="8.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="13" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13" style="42" customWidth="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1"/>
     <col min="18" max="18" width="7.28515625" customWidth="1"/>
   </cols>
@@ -633,17 +636,17 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33" t="s">
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32" t="s">
         <v>19</v>
       </c>
       <c r="O5" s="19"/>
-      <c r="P5" s="42"/>
+      <c r="P5" s="41"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
@@ -657,14 +660,14 @@
         <v>4</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="24" t="s">
+      <c r="M6" s="23" t="s">
         <v>24</v>
       </c>
       <c r="N6" s="2"/>
@@ -674,31 +677,31 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>1.2E-2</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
-      <c r="M7" s="24"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="2"/>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="C8" s="28"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="I8" s="29"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
-      <c r="M8" s="24"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="2"/>
       <c r="O8" s="5"/>
     </row>
@@ -712,7 +715,7 @@
       <c r="E9">
         <v>2048</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="24">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K9" s="4">
@@ -724,7 +727,7 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="24">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K10" s="4">
@@ -736,7 +739,7 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="24">
         <v>1.6E-2</v>
       </c>
       <c r="K11" s="4">
@@ -745,17 +748,17 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="41">
+      <c r="I12" s="40">
         <v>1.2E-2</v>
       </c>
       <c r="J12" s="15"/>
@@ -764,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="15"/>
-      <c r="M12" s="41"/>
+      <c r="M12" s="40"/>
       <c r="N12" s="15"/>
       <c r="O12" s="16"/>
     </row>
@@ -772,11 +775,11 @@
       <c r="B14" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="23"/>
+      <c r="I14" s="22"/>
       <c r="K14" s="19"/>
-      <c r="M14" s="23"/>
+      <c r="M14" s="22"/>
       <c r="O14" s="19"/>
-      <c r="P14" s="42"/>
+      <c r="P14" s="41"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -794,7 +797,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="12"/>
@@ -802,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="14"/>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="23" t="s">
         <v>24</v>
       </c>
       <c r="N15" s="12"/>
@@ -819,10 +822,10 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="23"/>
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="23"/>
       <c r="N16" s="2"/>
       <c r="O16" s="5"/>
       <c r="P16" s="43"/>
@@ -834,11 +837,11 @@
       <c r="E17" s="8">
         <v>2048</v>
       </c>
-      <c r="I17" s="26"/>
+      <c r="I17" s="25"/>
       <c r="K17" s="9"/>
-      <c r="M17" s="26"/>
+      <c r="M17" s="25"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="22"/>
+      <c r="P17" s="44"/>
     </row>
     <row r="18" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20"/>
@@ -848,23 +851,23 @@
       <c r="F18" s="15">
         <v>4</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="33">
         <v>0.26700000000000002</v>
       </c>
       <c r="K18" s="16"/>
-      <c r="M18" s="34">
-        <v>0.252</v>
+      <c r="M18" s="33">
+        <v>0.25600000000000001</v>
       </c>
       <c r="O18" s="16"/>
-      <c r="P18" s="37"/>
+      <c r="P18" s="45"/>
     </row>
     <row r="19" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="33"/>
       <c r="K19" s="16"/>
-      <c r="M19" s="34"/>
+      <c r="M19" s="33"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="37"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
@@ -877,17 +880,17 @@
       <c r="G20">
         <v>23</v>
       </c>
-      <c r="I20" s="27"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
-      <c r="M20" s="27">
-        <v>44.465000000000003</v>
+      <c r="M20" s="26">
+        <v>144</v>
       </c>
       <c r="N20" s="11"/>
       <c r="O20" s="11">
         <f>M20/$M$18</f>
-        <v>176.44841269841271</v>
+        <v>562.5</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -901,21 +904,21 @@
       <c r="G21">
         <v>23</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="26"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
-      <c r="M21" s="27">
+      <c r="M21" s="26">
         <v>218</v>
       </c>
       <c r="N21" s="11"/>
       <c r="O21" s="11">
         <f>M21/$M$18</f>
-        <v>865.07936507936506</v>
-      </c>
-      <c r="P21" s="11">
+        <v>851.5625</v>
+      </c>
+      <c r="P21" s="42">
         <f>M21/$M$20</f>
-        <v>4.9027324862251209</v>
+        <v>1.5138888888888888</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -928,29 +931,29 @@
       <c r="G22">
         <v>23</v>
       </c>
-      <c r="I22" s="27"/>
+      <c r="I22" s="26"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
-      <c r="M22" s="27">
-        <v>180</v>
+      <c r="M22" s="26">
+        <v>221</v>
       </c>
       <c r="N22" s="11"/>
       <c r="O22" s="11">
         <f>M22/$M$18</f>
-        <v>714.28571428571433</v>
-      </c>
-      <c r="P22" s="11">
+        <v>863.28125</v>
+      </c>
+      <c r="P22" s="42">
         <f>M22/$M$20</f>
-        <v>4.0481277409198242</v>
+        <v>1.5347222222222223</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="I23" s="27"/>
+      <c r="I23" s="26"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
-      <c r="M23" s="27"/>
+      <c r="M23" s="26"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
     </row>
@@ -961,27 +964,28 @@
       <c r="E24" s="8">
         <v>512</v>
       </c>
-      <c r="M24" s="26"/>
-      <c r="P24" s="22"/>
+      <c r="I24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="P24" s="44"/>
     </row>
     <row r="25" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="37">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="M25" s="38">
+      <c r="M25" s="37">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="P25" s="37"/>
+      <c r="P25" s="45"/>
     </row>
     <row r="26" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
-      <c r="I26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="P26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="P26" s="45"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
@@ -989,24 +993,24 @@
         <v>22</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="F27" s="35">
+      <c r="F27" s="34">
         <v>4</v>
       </c>
       <c r="G27" s="20">
         <v>23</v>
       </c>
       <c r="H27" s="20"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="36">
-        <v>3.25</v>
-      </c>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37">
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="35">
+        <v>9.7420000000000009</v>
+      </c>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36">
         <f>M27/$M$25</f>
-        <v>250</v>
+        <v>749.38461538461547</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
@@ -1020,7 +1024,7 @@
       <c r="G28">
         <v>23</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <v>10.555999999999999</v>
       </c>
       <c r="J28" s="11"/>
@@ -1029,17 +1033,17 @@
         <v>959.63636363636363</v>
       </c>
       <c r="L28" s="11"/>
-      <c r="M28" s="27">
-        <v>13.7</v>
+      <c r="M28" s="26">
+        <v>11.8</v>
       </c>
       <c r="N28" s="11"/>
       <c r="O28" s="11">
         <f>M28/$M$25</f>
-        <v>1053.8461538461538</v>
-      </c>
-      <c r="P28" s="11">
+        <v>907.69230769230774</v>
+      </c>
+      <c r="P28" s="42">
         <f>O28/$O$27</f>
-        <v>4.2153846153846155</v>
+        <v>1.211250256620817</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -1052,7 +1056,7 @@
       <c r="G29">
         <v>23</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="26">
         <v>7.0979999999999999</v>
       </c>
       <c r="J29" s="11"/>
@@ -1061,17 +1065,17 @@
         <v>645.27272727272725</v>
       </c>
       <c r="L29" s="11"/>
-      <c r="M29" s="27">
-        <v>8.5950000000000006</v>
+      <c r="M29" s="26">
+        <v>14.536</v>
       </c>
       <c r="N29" s="11"/>
       <c r="O29" s="11">
         <f>M29/$M$25</f>
-        <v>661.15384615384619</v>
-      </c>
-      <c r="P29" s="11">
+        <v>1118.1538461538462</v>
+      </c>
+      <c r="P29" s="42">
         <f>O29/$O$27</f>
-        <v>2.6446153846153848</v>
+        <v>1.4920960788339148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement box filter approximation of Gaussian filter.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ModelRelief\Relief\tests\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ModelRelief\Relief\tests\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Array Fill</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>SciPy: gaussian_filter(a, sigma, order=0, …)</t>
+  </si>
+  <si>
+    <t>GaussianBlur2</t>
+  </si>
+  <si>
+    <t>(7,7,9)</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -264,7 +270,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -287,12 +292,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -317,6 +316,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,9 +613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:P29"/>
+  <dimension ref="B5:Q31"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -616,39 +629,41 @@
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="23" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="13" style="42" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="39" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="23" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13" style="39" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:17" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="30" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32" t="s">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="41"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="38"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -660,52 +675,55 @@
         <v>4</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="L6" s="46"/>
+      <c r="N6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="2"/>
+      <c r="P6" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="I7" s="29">
+      <c r="I7" s="28">
         <v>1.2E-2</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="5"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L7" s="46"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="C8" s="27"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="I8" s="28"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="2"/>
       <c r="K8" s="5"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="46"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
@@ -715,7 +733,7 @@
       <c r="E9">
         <v>2048</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="23">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K9" s="4">
@@ -723,11 +741,11 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="23">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K10" s="4">
@@ -735,11 +753,11 @@
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="23">
         <v>1.6E-2</v>
       </c>
       <c r="K11" s="4">
@@ -747,41 +765,43 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="38" t="s">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="40">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="37">
         <v>1.2E-2</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16">
+      <c r="J12" s="14"/>
+      <c r="K12" s="15">
         <f>I12/$I$7</f>
         <v>1</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16"/>
-    </row>
-    <row r="14" spans="2:16" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="17" t="s">
+      <c r="L12" s="42"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="15"/>
+    </row>
+    <row r="14" spans="2:17" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="K14" s="19"/>
-      <c r="M14" s="22"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="41"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I14" s="21"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="38"/>
+      <c r="N14" s="21"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="38"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -797,24 +817,25 @@
         <v>20</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="12"/>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="23" t="s">
+      <c r="L15" s="46"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="12"/>
+      <c r="P15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P15" s="43"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="40"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -822,54 +843,58 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="43"/>
-    </row>
-    <row r="17" spans="2:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="L16" s="46"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="40"/>
+    </row>
+    <row r="17" spans="2:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="8">
         <v>2048</v>
       </c>
-      <c r="I17" s="25"/>
+      <c r="I17" s="24"/>
       <c r="K17" s="9"/>
-      <c r="M17" s="25"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="44"/>
-    </row>
-    <row r="18" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="15" t="s">
+      <c r="L17" s="41"/>
+      <c r="N17" s="24"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="41"/>
+    </row>
+    <row r="18" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>4</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="30">
         <v>0.26700000000000002</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="M18" s="33">
+      <c r="K18" s="15"/>
+      <c r="L18" s="42"/>
+      <c r="N18" s="30">
         <v>0.25600000000000001</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="45"/>
-    </row>
-    <row r="19" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="I19" s="33"/>
-      <c r="K19" s="16"/>
-      <c r="M19" s="33"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="45"/>
-    </row>
-    <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="15"/>
+      <c r="Q18" s="42"/>
+    </row>
+    <row r="19" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="19"/>
+      <c r="I19" s="30"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="42"/>
+      <c r="N19" s="30"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="42"/>
+    </row>
+    <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" t="s">
         <v>22</v>
@@ -880,20 +905,25 @@
       <c r="G20">
         <v>23</v>
       </c>
-      <c r="I20" s="26"/>
+      <c r="I20" s="25">
+        <v>123</v>
+      </c>
       <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="26">
+      <c r="K20" s="11">
+        <f t="shared" ref="K20:K22" si="0">I20/$I$18</f>
+        <v>460.67415730337075</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="25">
         <v>144</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11">
-        <f>M20/$M$18</f>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11">
+        <f>N20/$N$18</f>
         <v>562.5</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" t="s">
         <v>14</v>
@@ -904,24 +934,33 @@
       <c r="G21">
         <v>23</v>
       </c>
-      <c r="I21" s="26"/>
+      <c r="I21" s="25">
+        <v>171</v>
+      </c>
       <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="26">
+      <c r="K21" s="11">
+        <f t="shared" si="0"/>
+        <v>640.44943820224717</v>
+      </c>
+      <c r="L21" s="39">
+        <f>K21/$K$20</f>
+        <v>1.3902439024390245</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="25">
         <v>218</v>
       </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11">
-        <f>M21/$M$18</f>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11">
+        <f>N21/$N$18</f>
         <v>851.5625</v>
       </c>
-      <c r="P21" s="42">
-        <f>M21/$M$20</f>
+      <c r="Q21" s="39">
+        <f>N21/$N$20</f>
         <v>1.5138888888888888</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>17</v>
       </c>
@@ -931,124 +970,136 @@
       <c r="G22">
         <v>23</v>
       </c>
-      <c r="I22" s="26"/>
+      <c r="I22" s="25">
+        <v>185</v>
+      </c>
       <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="26">
+      <c r="K22" s="11">
+        <f t="shared" si="0"/>
+        <v>692.88389513108609</v>
+      </c>
+      <c r="L22" s="39">
+        <f>K22/$K$20</f>
+        <v>1.5040650406504066</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="25">
         <v>221</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11">
-        <f>M22/$M$18</f>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11">
+        <f>N22/$N$18</f>
         <v>863.28125</v>
       </c>
-      <c r="P22" s="42">
-        <f>M22/$M$20</f>
+      <c r="Q22" s="39">
+        <f>N22/$N$20</f>
         <v>1.5347222222222223</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="I23" s="26"/>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="25">
+        <v>155</v>
+      </c>
       <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="11"/>
+      <c r="K23" s="11">
+        <f>I23/$I$18</f>
+        <v>580.52434456928836</v>
+      </c>
+      <c r="L23" s="39">
+        <f>K23/$K$20</f>
+        <v>1.2601626016260163</v>
+      </c>
+      <c r="M23" s="11"/>
+      <c r="N23" s="25"/>
       <c r="O23" s="11"/>
-    </row>
-    <row r="24" spans="2:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="P23" s="11"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I24" s="25"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+    </row>
+    <row r="25" spans="2:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E25" s="8">
         <v>512</v>
       </c>
-      <c r="I24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="P24" s="44"/>
-    </row>
-    <row r="25" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="15" t="s">
+      <c r="I25" s="24"/>
+      <c r="L25" s="41"/>
+      <c r="N25" s="24"/>
+      <c r="Q25" s="41"/>
+    </row>
+    <row r="26" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="19"/>
+      <c r="C26" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="37">
+      <c r="I26" s="34">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="M25" s="37">
+      <c r="L26" s="42"/>
+      <c r="N26" s="34">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="P25" s="45"/>
-    </row>
-    <row r="26" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="I26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="P26" s="45"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="F27" s="34">
-        <v>4</v>
-      </c>
-      <c r="G27" s="20">
-        <v>23</v>
-      </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="35">
-        <v>9.7420000000000009</v>
-      </c>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36">
-        <f>M27/$M$25</f>
-        <v>749.38461538461547</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="42"/>
+    </row>
+    <row r="27" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="19"/>
+      <c r="I27" s="34"/>
+      <c r="L27" s="42"/>
+      <c r="N27" s="34"/>
+      <c r="Q27" s="42"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="F28" s="31">
+        <v>4</v>
+      </c>
+      <c r="G28" s="19">
+        <v>23</v>
+      </c>
+      <c r="H28" s="19"/>
+      <c r="I28" s="32">
+        <v>8</v>
+      </c>
+      <c r="J28" s="33"/>
+      <c r="K28" s="11">
+        <f t="shared" ref="K28:K30" si="1">I28/$I$26</f>
+        <v>727.27272727272737</v>
+      </c>
+      <c r="M28" s="33"/>
+      <c r="N28" s="32">
+        <v>9.7420000000000009</v>
+      </c>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33">
+        <f>N28/$N$26</f>
+        <v>749.38461538461547</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" t="s">
         <v>14</v>
-      </c>
-      <c r="F28">
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <v>23</v>
-      </c>
-      <c r="I28" s="26">
-        <v>10.555999999999999</v>
-      </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11">
-        <f>I28/$I$25</f>
-        <v>959.63636363636363</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="26">
-        <v>11.8</v>
-      </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11">
-        <f>M28/$M$25</f>
-        <v>907.69230769230774</v>
-      </c>
-      <c r="P28" s="42">
-        <f>O28/$O$27</f>
-        <v>1.211250256620817</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>17</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -1056,31 +1107,98 @@
       <c r="G29">
         <v>23</v>
       </c>
-      <c r="I29" s="26">
-        <v>7.0979999999999999</v>
+      <c r="I29" s="25">
+        <v>10.5</v>
       </c>
       <c r="J29" s="11"/>
       <c r="K29" s="11">
-        <f>I29/$I$25</f>
-        <v>645.27272727272725</v>
-      </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="26">
+        <f t="shared" si="1"/>
+        <v>954.54545454545462</v>
+      </c>
+      <c r="L29" s="39">
+        <f>K29/$K$28</f>
+        <v>1.3125</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="25">
+        <v>11.8</v>
+      </c>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11">
+        <f>N29/$N$26</f>
+        <v>907.69230769230774</v>
+      </c>
+      <c r="Q29" s="39">
+        <f>P29/$P$28</f>
+        <v>1.211250256620817</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+      <c r="I30" s="25">
+        <v>11.5</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11">
+        <f t="shared" si="1"/>
+        <v>1045.4545454545455</v>
+      </c>
+      <c r="L30" s="39">
+        <f>K30/$K$28</f>
+        <v>1.4374999999999998</v>
+      </c>
+      <c r="M30" s="11"/>
+      <c r="N30" s="25">
         <v>14.536</v>
       </c>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11">
-        <f>M29/$M$25</f>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11">
+        <f>N30/$N$26</f>
         <v>1118.1538461538462</v>
       </c>
-      <c r="P29" s="42">
-        <f>O29/$O$27</f>
+      <c r="Q30" s="39">
+        <f>P30/$P$28</f>
         <v>1.4920960788339148</v>
       </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="25">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11">
+        <f>I31/$I$26</f>
+        <v>890.90909090909099</v>
+      </c>
+      <c r="L31" s="39">
+        <f>K31/$K$28</f>
+        <v>1.2249999999999999</v>
+      </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rename Gaussian methods to reflect underlying algorithms.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -117,18 +117,12 @@
     </r>
   </si>
   <si>
-    <t>GaussianBlur1</t>
-  </si>
-  <si>
     <t>benchmark (2048, 2048)</t>
   </si>
   <si>
     <t>Explorer (512, 512)</t>
   </si>
   <si>
-    <t>GaussianBlur1A</t>
-  </si>
-  <si>
     <t>Vector</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>Sigma</t>
   </si>
   <si>
-    <t>GaussianFilter.ApplyKernel</t>
-  </si>
-  <si>
     <t>SciPy: a[:] = value</t>
   </si>
   <si>
@@ -153,10 +144,19 @@
     <t>SciPy: gaussian_filter(a, sigma, order=0, …)</t>
   </si>
   <si>
-    <t>GaussianBlur2</t>
-  </si>
-  <si>
     <t>(5, 5, 7, 7, 7)</t>
+  </si>
+  <si>
+    <t>GaussianFilter</t>
+  </si>
+  <si>
+    <t>GaussianBlur</t>
+  </si>
+  <si>
+    <t>GaussianBlurBox</t>
+  </si>
+  <si>
+    <t>GaussianBlurBoxIndependent</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="B5:Q31"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,14 +651,14 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="43"/>
       <c r="L5" s="43"/>
       <c r="M5" s="44"/>
       <c r="N5" s="29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P5" s="18"/>
       <c r="Q5" s="38"/>
@@ -676,7 +676,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="I6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="5" t="s">
@@ -684,7 +684,7 @@
       </c>
       <c r="L6" s="46"/>
       <c r="N6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="5" t="s">
@@ -694,7 +694,7 @@
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -811,14 +811,14 @@
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="5" t="s">
@@ -827,7 +827,7 @@
       <c r="L15" s="46"/>
       <c r="M15" s="13"/>
       <c r="N15" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="5" t="s">
@@ -854,7 +854,7 @@
     </row>
     <row r="17" spans="2:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8">
         <v>2048</v>
@@ -869,7 +869,7 @@
     <row r="18" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18" s="14">
         <v>4</v>
@@ -897,7 +897,7 @@
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -926,7 +926,7 @@
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F21">
         <v>4</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F22">
         <v>4</v>
@@ -998,13 +998,13 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
       <c r="G23" s="45" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I23" s="25">
         <v>179</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="25" spans="2:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="8">
         <v>512</v>
@@ -1047,7 +1047,7 @@
     <row r="26" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
       <c r="C26" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I26" s="34">
         <v>1.0999999999999999E-2</v>
@@ -1068,7 +1068,7 @@
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D28" s="14"/>
       <c r="F28" s="31">
@@ -1079,12 +1079,12 @@
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="32">
-        <v>8</v>
+        <v>8.9</v>
       </c>
       <c r="J28" s="33"/>
       <c r="K28" s="11">
         <f t="shared" ref="K28:K30" si="1">I28/$I$26</f>
-        <v>727.27272727272737</v>
+        <v>809.09090909090912</v>
       </c>
       <c r="M28" s="33"/>
       <c r="N28" s="32">
@@ -1099,7 +1099,7 @@
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -1108,16 +1108,16 @@
         <v>23</v>
       </c>
       <c r="I29" s="25">
-        <v>10.5</v>
+        <v>11.016999999999999</v>
       </c>
       <c r="J29" s="11"/>
       <c r="K29" s="11">
         <f t="shared" si="1"/>
-        <v>954.54545454545462</v>
+        <v>1001.5454545454545</v>
       </c>
       <c r="L29" s="39">
         <f>K29/$K$28</f>
-        <v>1.3125</v>
+        <v>1.2378651685393258</v>
       </c>
       <c r="M29" s="11"/>
       <c r="N29" s="25">
@@ -1135,7 +1135,7 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F30">
         <v>4</v>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="L30" s="39">
         <f>K30/$K$28</f>
-        <v>1.4374999999999998</v>
+        <v>1.2921348314606742</v>
       </c>
       <c r="M30" s="11"/>
       <c r="N30" s="25">
@@ -1171,25 +1171,25 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" s="45" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I31" s="25">
-        <v>12.3</v>
+        <v>11.3</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11">
         <f>I31/$I$26</f>
-        <v>1118.1818181818182</v>
+        <v>1027.2727272727275</v>
       </c>
       <c r="L31" s="39">
         <f>K31/$K$28</f>
-        <v>1.5374999999999999</v>
+        <v>1.2696629213483148</v>
       </c>
       <c r="M31" s="11"/>
       <c r="N31" s="25"/>

</xml_diff>

<commit_message>
Convert gaussian filter methods to 'constant' from 'reflect'.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -690,7 +690,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="M33" sqref="M33:M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,13 +953,11 @@
         <v>460.67415730337075</v>
       </c>
       <c r="L14" s="11"/>
-      <c r="M14" s="24">
-        <v>144</v>
-      </c>
+      <c r="M14" s="24"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11">
         <f>M14/$M$13</f>
-        <v>562.5</v>
+        <v>0</v>
       </c>
       <c r="P14" s="38"/>
       <c r="Q14" s="35"/>
@@ -997,13 +995,11 @@
         <v>640.44943820224717</v>
       </c>
       <c r="L16" s="43"/>
-      <c r="M16" s="50">
-        <v>218</v>
-      </c>
+      <c r="M16" s="50"/>
       <c r="N16" s="43"/>
       <c r="O16" s="43">
         <f>M16/$M$13</f>
-        <v>851.5625</v>
+        <v>0</v>
       </c>
       <c r="P16" s="40"/>
     </row>
@@ -1030,13 +1026,11 @@
         <v>692.88389513108609</v>
       </c>
       <c r="L17" s="43"/>
-      <c r="M17" s="50">
-        <v>221</v>
-      </c>
+      <c r="M17" s="50"/>
       <c r="N17" s="43"/>
       <c r="O17" s="43">
         <f>M17/$M$13</f>
-        <v>863.28125</v>
+        <v>0</v>
       </c>
       <c r="P17" s="40"/>
     </row>
@@ -1156,13 +1150,13 @@
       </c>
       <c r="H23"/>
       <c r="I23" s="47">
-        <f>19.612/4</f>
-        <v>4.9029999999999996</v>
+        <f>18.846/4</f>
+        <v>4.7115</v>
       </c>
       <c r="J23" s="11"/>
       <c r="K23" s="11">
         <f>I23/$I$22</f>
-        <v>784.4799999999999</v>
+        <v>753.83999999999992</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="24">
@@ -1201,13 +1195,13 @@
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="49">
-        <f>24.91/4</f>
-        <v>6.2275</v>
+        <f>24.748/4</f>
+        <v>6.1870000000000003</v>
       </c>
       <c r="J25" s="43"/>
       <c r="K25" s="43">
         <f>I25/$I$22</f>
-        <v>996.4</v>
+        <v>989.92</v>
       </c>
       <c r="L25" s="43"/>
       <c r="M25" s="50">
@@ -1235,13 +1229,13 @@
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="49">
-        <f>28.39/4</f>
-        <v>7.0975000000000001</v>
+        <f>28.199/4</f>
+        <v>7.0497500000000004</v>
       </c>
       <c r="J26" s="43"/>
       <c r="K26" s="43">
         <f>I26/$I$22</f>
-        <v>1135.5999999999999</v>
+        <v>1127.96</v>
       </c>
       <c r="L26" s="43"/>
       <c r="M26" s="50">
@@ -1297,13 +1291,13 @@
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="50">
-        <f>27.095/4</f>
-        <v>6.7737499999999997</v>
+        <f>26.747/4</f>
+        <v>6.68675</v>
       </c>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
         <f>I28/$I$22</f>
-        <v>1083.8</v>
+        <v>1069.8799999999999</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1390,21 +1384,19 @@
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="30">
-        <v>8.9</v>
+        <v>7.758</v>
       </c>
       <c r="J33" s="31"/>
       <c r="K33" s="11">
         <f t="shared" ref="K33:K36" si="1">I33/$I$32</f>
-        <v>809.09090909090912</v>
+        <v>705.27272727272737</v>
       </c>
       <c r="L33" s="31"/>
-      <c r="M33" s="30">
-        <v>9.7420000000000009</v>
-      </c>
+      <c r="M33" s="30"/>
       <c r="N33" s="31"/>
       <c r="O33" s="31">
         <f>M33/$M$32</f>
-        <v>749.38461538461547</v>
+        <v>0</v>
       </c>
       <c r="P33" s="38"/>
       <c r="Q33" s="35"/>
@@ -1438,21 +1430,19 @@
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="50">
-        <v>11.016999999999999</v>
+        <v>10.157</v>
       </c>
       <c r="J35" s="43"/>
       <c r="K35" s="43">
         <f t="shared" si="1"/>
-        <v>1001.5454545454545</v>
+        <v>923.36363636363637</v>
       </c>
       <c r="L35" s="43"/>
-      <c r="M35" s="50">
-        <v>11.8</v>
-      </c>
+      <c r="M35" s="50"/>
       <c r="N35" s="43"/>
       <c r="O35" s="43">
         <f>M35/$M$32</f>
-        <v>907.69230769230774</v>
+        <v>0</v>
       </c>
       <c r="P35" s="40"/>
     </row>
@@ -1471,21 +1461,19 @@
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="50">
-        <v>11.5</v>
+        <v>11.526</v>
       </c>
       <c r="J36" s="43"/>
       <c r="K36" s="43">
         <f t="shared" si="1"/>
-        <v>1045.4545454545455</v>
+        <v>1047.8181818181818</v>
       </c>
       <c r="L36" s="43"/>
-      <c r="M36" s="50">
-        <v>14.536</v>
-      </c>
+      <c r="M36" s="50"/>
       <c r="N36" s="43"/>
       <c r="O36" s="43">
         <f>M36/$M$32</f>
-        <v>1118.1538461538462</v>
+        <v>0</v>
       </c>
       <c r="P36" s="40"/>
     </row>
@@ -1503,12 +1491,12 @@
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="50">
-        <v>11.3</v>
+        <v>10.97</v>
       </c>
       <c r="J37" s="43"/>
       <c r="K37" s="43">
         <f>I37/$I$32</f>
-        <v>1027.2727272727275</v>
+        <v>997.27272727272737</v>
       </c>
       <c r="L37" s="43"/>
       <c r="M37" s="50"/>

</xml_diff>

<commit_message>
Optimize GaussianBlurCachedKernel by replacing min, max.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Array Fill</t>
   </si>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33:M36"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,9 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D23"/>
+      <c r="D23" s="34" t="s">
+        <v>10</v>
+      </c>
       <c r="E23"/>
       <c r="F23">
         <v>4</v>
@@ -1150,13 +1152,13 @@
       </c>
       <c r="H23"/>
       <c r="I23" s="47">
-        <f>18.846/4</f>
-        <v>4.7115</v>
+        <f>18.554/4</f>
+        <v>4.6384999999999996</v>
       </c>
       <c r="J23" s="11"/>
       <c r="K23" s="11">
         <f>I23/$I$22</f>
-        <v>753.83999999999992</v>
+        <v>742.15999999999985</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="24">
@@ -1185,7 +1187,9 @@
       <c r="C25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8">
         <v>4</v>
@@ -1195,13 +1199,13 @@
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="49">
-        <f>24.748/4</f>
-        <v>6.1870000000000003</v>
+        <f>24.182/4</f>
+        <v>6.0454999999999997</v>
       </c>
       <c r="J25" s="43"/>
       <c r="K25" s="43">
         <f>I25/$I$22</f>
-        <v>989.92</v>
+        <v>967.27999999999986</v>
       </c>
       <c r="L25" s="43"/>
       <c r="M25" s="50">
@@ -1219,7 +1223,9 @@
       <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8">
         <v>4</v>
@@ -1229,13 +1235,13 @@
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="49">
-        <f>28.199/4</f>
-        <v>7.0497500000000004</v>
+        <f>1.964/4</f>
+        <v>0.49099999999999999</v>
       </c>
       <c r="J26" s="43"/>
       <c r="K26" s="43">
         <f>I26/$I$22</f>
-        <v>1127.96</v>
+        <v>78.559999999999988</v>
       </c>
       <c r="L26" s="43"/>
       <c r="M26" s="50">
@@ -1290,14 +1296,11 @@
         <v>23</v>
       </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="50">
-        <f>26.747/4</f>
-        <v>6.68675</v>
-      </c>
+      <c r="I28" s="50"/>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
         <f>I28/$I$22</f>
-        <v>1069.8799999999999</v>
+        <v>0</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1383,13 +1386,13 @@
         <v>23</v>
       </c>
       <c r="H33" s="19"/>
-      <c r="I33" s="30">
-        <v>7.758</v>
+      <c r="I33" s="47">
+        <v>8.1280000000000001</v>
       </c>
       <c r="J33" s="31"/>
       <c r="K33" s="11">
         <f t="shared" ref="K33:K36" si="1">I33/$I$32</f>
-        <v>705.27272727272737</v>
+        <v>738.90909090909099</v>
       </c>
       <c r="L33" s="31"/>
       <c r="M33" s="30"/>
@@ -1407,7 +1410,7 @@
       <c r="F34" s="29"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
-      <c r="I34" s="30"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="31"/>
       <c r="K34" s="11"/>
       <c r="L34" s="31"/>
@@ -1429,13 +1432,13 @@
         <v>23</v>
       </c>
       <c r="H35" s="8"/>
-      <c r="I35" s="50">
-        <v>10.157</v>
+      <c r="I35" s="49">
+        <v>10.641</v>
       </c>
       <c r="J35" s="43"/>
       <c r="K35" s="43">
         <f t="shared" si="1"/>
-        <v>923.36363636363637</v>
+        <v>967.36363636363637</v>
       </c>
       <c r="L35" s="43"/>
       <c r="M35" s="50"/>
@@ -1460,13 +1463,13 @@
         <v>23</v>
       </c>
       <c r="H36" s="8"/>
-      <c r="I36" s="50">
-        <v>11.526</v>
+      <c r="I36" s="49">
+        <v>0.89200000000000002</v>
       </c>
       <c r="J36" s="43"/>
       <c r="K36" s="43">
         <f t="shared" si="1"/>
-        <v>1047.8181818181818</v>
+        <v>81.090909090909093</v>
       </c>
       <c r="L36" s="43"/>
       <c r="M36" s="50"/>
@@ -1490,13 +1493,11 @@
         <v>23</v>
       </c>
       <c r="H37" s="8"/>
-      <c r="I37" s="50">
-        <v>10.97</v>
-      </c>
+      <c r="I37" s="49"/>
       <c r="J37" s="43"/>
       <c r="K37" s="43">
         <f>I37/$I$32</f>
-        <v>997.27272727272737</v>
+        <v>0</v>
       </c>
       <c r="L37" s="43"/>
       <c r="M37" s="50"/>
@@ -1517,7 +1518,7 @@
         <v>29</v>
       </c>
       <c r="H38" s="8"/>
-      <c r="I38" s="23"/>
+      <c r="I38" s="49"/>
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
       <c r="L38" s="8"/>
@@ -1535,7 +1536,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="23"/>
+      <c r="I39" s="49"/>
       <c r="J39" s="8"/>
       <c r="K39" s="9"/>
       <c r="L39" s="8"/>

</xml_diff>

<commit_message>
Complete implementation of GaussianBlurBox.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -690,7 +690,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,11 +1296,14 @@
         <v>23</v>
       </c>
       <c r="H28" s="8"/>
-      <c r="I28" s="50"/>
+      <c r="I28" s="49">
+        <f>0.676/4</f>
+        <v>0.16900000000000001</v>
+      </c>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
         <f>I28/$I$22</f>
-        <v>0</v>
+        <v>27.04</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1321,7 +1324,7 @@
         <v>23</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="I29" s="50"/>
+      <c r="I29" s="49"/>
       <c r="J29" s="43"/>
       <c r="K29" s="43"/>
       <c r="L29" s="43"/>
@@ -1339,7 +1342,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="50"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="43"/>
       <c r="K30" s="43"/>
       <c r="L30" s="43"/>
@@ -1493,11 +1496,13 @@
         <v>23</v>
       </c>
       <c r="H37" s="8"/>
-      <c r="I37" s="49"/>
+      <c r="I37" s="49">
+        <v>0.28899999999999998</v>
+      </c>
       <c r="J37" s="43"/>
       <c r="K37" s="43">
         <f>I37/$I$32</f>
-        <v>0</v>
+        <v>26.272727272727273</v>
       </c>
       <c r="L37" s="43"/>
       <c r="M37" s="50"/>

</xml_diff>

<commit_message>
Complete implementation of GaussianBlurBoxIndependent.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -690,7 +690,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,9 +1324,15 @@
         <v>23</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="I29" s="49"/>
+      <c r="I29" s="49">
+        <f>0.174/4</f>
+        <v>4.3499999999999997E-2</v>
+      </c>
       <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
+      <c r="K29" s="43">
+        <f>I29/$I$22</f>
+        <v>6.9599999999999991</v>
+      </c>
       <c r="L29" s="43"/>
       <c r="M29" s="50"/>
       <c r="N29" s="43"/>
@@ -1523,9 +1529,14 @@
         <v>29</v>
       </c>
       <c r="H38" s="8"/>
-      <c r="I38" s="49"/>
+      <c r="I38" s="49">
+        <v>7.2999999999999995E-2</v>
+      </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="9"/>
+      <c r="K38" s="43">
+        <f>I38/$I$32</f>
+        <v>6.6363636363636367</v>
+      </c>
       <c r="L38" s="8"/>
       <c r="M38" s="23"/>
       <c r="N38" s="8"/>

</xml_diff>

<commit_message>
Update Gaussian benchmark results.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -178,7 +178,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -268,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -359,6 +360,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,9 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
-    </sheetView>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -920,7 +920,8 @@
         <v>4</v>
       </c>
       <c r="I13" s="46">
-        <v>0.26700000000000002</v>
+        <f>1.16/4</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K13" s="15"/>
       <c r="M13" s="28">
@@ -945,12 +946,13 @@
       </c>
       <c r="H14"/>
       <c r="I14" s="24">
-        <v>123</v>
+        <f>500/4</f>
+        <v>125</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="11">
         <f t="shared" ref="K14:K17" si="0">I14/$I$13</f>
-        <v>460.67415730337075</v>
+        <v>431.0344827586207</v>
       </c>
       <c r="L14" s="11"/>
       <c r="M14" s="24"/>
@@ -986,13 +988,14 @@
         <v>23</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="50">
-        <v>171</v>
+      <c r="I16" s="52">
+        <f>651/4</f>
+        <v>162.75</v>
       </c>
       <c r="J16" s="43"/>
       <c r="K16" s="43">
         <f t="shared" si="0"/>
-        <v>640.44943820224717</v>
+        <v>561.20689655172418</v>
       </c>
       <c r="L16" s="43"/>
       <c r="M16" s="50"/>
@@ -1017,13 +1020,14 @@
         <v>23</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="50">
-        <v>185</v>
+      <c r="I17" s="52">
+        <f>55.791/4</f>
+        <v>13.947749999999999</v>
       </c>
       <c r="J17" s="43"/>
       <c r="K17" s="43">
         <f t="shared" si="0"/>
-        <v>692.88389513108609</v>
+        <v>48.095689655172414</v>
       </c>
       <c r="L17" s="43"/>
       <c r="M17" s="50"/>
@@ -1047,13 +1051,14 @@
         <v>23</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="50">
-        <v>179</v>
+      <c r="I18" s="52">
+        <f>15.845/4</f>
+        <v>3.9612500000000002</v>
       </c>
       <c r="J18" s="43"/>
       <c r="K18" s="43">
         <f>I18/$I$13</f>
-        <v>670.41198501872657</v>
+        <v>13.65948275862069</v>
       </c>
       <c r="L18" s="43"/>
       <c r="M18" s="50"/>
@@ -1074,9 +1079,15 @@
         <v>23</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="50"/>
+      <c r="I19" s="52">
+        <f>4.617/4</f>
+        <v>1.15425</v>
+      </c>
       <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
+      <c r="K19" s="43">
+        <f>I19/$I$13</f>
+        <v>3.9801724137931038</v>
+      </c>
       <c r="L19" s="43"/>
       <c r="M19" s="50"/>
       <c r="N19" s="43"/>
@@ -1092,7 +1103,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="50"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="43"/>
       <c r="K20" s="43"/>
       <c r="L20" s="43"/>

</xml_diff>

<commit_message>
Update Gaussian benchmark times.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Array Fill</t>
   </si>
@@ -691,7 +691,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1100,12 +1102,22 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="8">
+        <v>4</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="52"/>
+      <c r="I20" s="52">
+        <f>5.593/4</f>
+        <v>1.39825</v>
+      </c>
       <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="K20" s="43">
+        <f>I20/$I$13</f>
+        <v>4.8215517241379313</v>
+      </c>
       <c r="L20" s="43"/>
       <c r="M20" s="50"/>
       <c r="N20" s="43"/>
@@ -1163,13 +1175,13 @@
       </c>
       <c r="H23"/>
       <c r="I23" s="47">
-        <f>18.554/4</f>
-        <v>4.6384999999999996</v>
+        <f>19.617/4</f>
+        <v>4.9042500000000002</v>
       </c>
       <c r="J23" s="11"/>
       <c r="K23" s="11">
         <f>I23/$I$22</f>
-        <v>742.15999999999985</v>
+        <v>784.68</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="24">
@@ -1210,13 +1222,13 @@
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="49">
-        <f>24.182/4</f>
-        <v>6.0454999999999997</v>
+        <f>25.726/4</f>
+        <v>6.4314999999999998</v>
       </c>
       <c r="J25" s="43"/>
       <c r="K25" s="43">
         <f>I25/$I$22</f>
-        <v>967.27999999999986</v>
+        <v>1029.04</v>
       </c>
       <c r="L25" s="43"/>
       <c r="M25" s="50">
@@ -1246,13 +1258,13 @@
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="49">
-        <f>1.964/4</f>
-        <v>0.49099999999999999</v>
+        <f>2.005/4</f>
+        <v>0.50124999999999997</v>
       </c>
       <c r="J26" s="43"/>
       <c r="K26" s="43">
         <f>I26/$I$22</f>
-        <v>78.559999999999988</v>
+        <v>80.199999999999989</v>
       </c>
       <c r="L26" s="43"/>
       <c r="M26" s="50">
@@ -1270,7 +1282,9 @@
       <c r="C27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8">
         <v>4</v>
@@ -1298,7 +1312,9 @@
       <c r="C28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8">
         <v>4</v>
@@ -1308,13 +1324,13 @@
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="49">
-        <f>0.676/4</f>
-        <v>0.16900000000000001</v>
+        <f>0.731/4</f>
+        <v>0.18275</v>
       </c>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
         <f>I28/$I$22</f>
-        <v>27.04</v>
+        <v>29.24</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1326,7 +1342,9 @@
       <c r="C29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8">
         <v>4</v>
@@ -1336,13 +1354,13 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="49">
-        <f>0.174/4</f>
-        <v>4.3499999999999997E-2</v>
+        <f>0.164/4</f>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J29" s="43"/>
       <c r="K29" s="43">
         <f>I29/$I$22</f>
-        <v>6.9599999999999991</v>
+        <v>6.56</v>
       </c>
       <c r="L29" s="43"/>
       <c r="M29" s="50"/>
@@ -1354,14 +1372,26 @@
       <c r="C30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="F30" s="8">
+        <v>4</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="H30" s="8"/>
-      <c r="I30" s="49"/>
+      <c r="I30" s="49">
+        <f>0.114/4</f>
+        <v>2.8500000000000001E-2</v>
+      </c>
       <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
+      <c r="K30" s="43">
+        <f>I30/$I$22</f>
+        <v>4.5599999999999996</v>
+      </c>
       <c r="L30" s="43"/>
       <c r="M30" s="50"/>
       <c r="N30" s="43"/>
@@ -1537,7 +1567,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="44" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="49">
@@ -1560,12 +1590,21 @@
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
+      <c r="F39" s="8">
+        <v>4</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="H39" s="8"/>
-      <c r="I39" s="49"/>
+      <c r="I39" s="49">
+        <v>6.7000000000000004E-2</v>
+      </c>
       <c r="J39" s="8"/>
-      <c r="K39" s="9"/>
+      <c r="K39" s="43">
+        <f>I39/$I$32</f>
+        <v>6.0909090909090917</v>
+      </c>
       <c r="L39" s="8"/>
       <c r="M39" s="23"/>
       <c r="N39" s="8"/>

</xml_diff>

<commit_message>
Rename Gaussian blur methods.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>Array Fill</t>
   </si>
@@ -147,31 +147,28 @@
     <t>(5, 5, 7, 7, 7)</t>
   </si>
   <si>
-    <t>GaussianFilter</t>
-  </si>
-  <si>
-    <t>GaussianBlur</t>
-  </si>
-  <si>
-    <t>GaussianBlurBox</t>
-  </si>
-  <si>
-    <t>GaussianBlurBoxIndependent</t>
-  </si>
-  <si>
-    <t>GaussianBlurCachedKernel</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>benchmark (400, 400)</t>
   </si>
   <si>
-    <t>GaussianBlurBoxIndependentOptimized</t>
-  </si>
-  <si>
-    <t>GaussianBlurCachedKernel: NOOP</t>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>GaussianCached</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>BoxIndependent</t>
+  </si>
+  <si>
+    <t>BoxIndependentDelta</t>
   </si>
 </sst>
 </file>
@@ -689,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +933,7 @@
     <row r="14" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -979,7 +976,7 @@
     <row r="16" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1042,7 +1039,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1070,7 +1067,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1135,10 +1132,10 @@
     </row>
     <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>22</v>
@@ -1161,7 +1158,7 @@
     <row r="23" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>10</v>
@@ -1208,7 +1205,7 @@
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>10</v>
@@ -1278,9 +1275,8 @@
       <c r="P26" s="40"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
       <c r="C27" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>10</v>
@@ -1289,18 +1285,18 @@
       <c r="F27" s="8">
         <v>4</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="49">
-        <f>0.484/4</f>
-        <v>0.121</v>
+        <f>0.731/4</f>
+        <v>0.18275</v>
       </c>
       <c r="J27" s="43"/>
       <c r="K27" s="43">
         <f>I27/$I$22</f>
-        <v>19.36</v>
+        <v>29.24</v>
       </c>
       <c r="L27" s="43"/>
       <c r="M27" s="50"/>
@@ -1310,7 +1306,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>10</v>
@@ -1324,13 +1320,13 @@
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="49">
-        <f>0.731/4</f>
-        <v>0.18275</v>
+        <f>0.164/4</f>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
         <f>I28/$I$22</f>
-        <v>29.24</v>
+        <v>6.56</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1340,7 +1336,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>10</v>
@@ -1354,13 +1350,13 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="49">
-        <f>0.164/4</f>
-        <v>4.1000000000000002E-2</v>
+        <f>0.114/4</f>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="J29" s="43"/>
       <c r="K29" s="43">
         <f>I29/$I$22</f>
-        <v>6.56</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="L29" s="43"/>
       <c r="M29" s="50"/>
@@ -1369,109 +1365,110 @@
       <c r="P29" s="40"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8">
-        <v>4</v>
-      </c>
-      <c r="G30" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="49">
-        <f>0.114/4</f>
-        <v>2.8500000000000001E-2</v>
-      </c>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43">
-        <f>I30/$I$22</f>
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="40"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I31" s="24"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+    </row>
+    <row r="31" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="51">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="M31" s="32">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="35"/>
     </row>
     <row r="32" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="51">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="M32" s="32">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="P32" s="39"/>
+      <c r="B32" s="19"/>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" s="29">
+        <v>4</v>
+      </c>
+      <c r="G32" s="19">
+        <v>23</v>
+      </c>
+      <c r="H32" s="19"/>
+      <c r="I32" s="47">
+        <v>8.1280000000000001</v>
+      </c>
+      <c r="J32" s="31"/>
+      <c r="K32" s="11">
+        <f t="shared" ref="K32:K35" si="1">I32/$I$31</f>
+        <v>738.90909090909099</v>
+      </c>
+      <c r="L32" s="31"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31">
+        <f>M32/$M$31</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="38"/>
       <c r="Q32" s="35"/>
     </row>
-    <row r="33" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33"/>
-      <c r="F33" s="29">
-        <v>4</v>
-      </c>
-      <c r="G33" s="19">
-        <v>23</v>
-      </c>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="D33" s="14"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="19"/>
       <c r="H33" s="19"/>
-      <c r="I33" s="47">
-        <v>8.1280000000000001</v>
-      </c>
+      <c r="I33" s="47"/>
       <c r="J33" s="31"/>
-      <c r="K33" s="11">
-        <f t="shared" ref="K33:K36" si="1">I33/$I$32</f>
-        <v>738.90909090909099</v>
-      </c>
+      <c r="K33" s="11"/>
       <c r="L33" s="31"/>
       <c r="M33" s="30"/>
       <c r="N33" s="31"/>
-      <c r="O33" s="31">
-        <f>M33/$M$32</f>
+      <c r="O33" s="31"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8">
+        <v>4</v>
+      </c>
+      <c r="G34" s="8">
+        <v>23</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="49">
+        <v>10.641</v>
+      </c>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43">
+        <f t="shared" si="1"/>
+        <v>967.36363636363637</v>
+      </c>
+      <c r="L34" s="43"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43">
+        <f>M34/$M$31</f>
         <v>0</v>
       </c>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="35"/>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="D34" s="14"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="40"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1483,56 +1480,52 @@
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="49">
-        <v>10.641</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="J35" s="43"/>
       <c r="K35" s="43">
         <f t="shared" si="1"/>
-        <v>967.36363636363637</v>
+        <v>81.090909090909093</v>
       </c>
       <c r="L35" s="43"/>
       <c r="M35" s="50"/>
       <c r="N35" s="43"/>
       <c r="O35" s="43">
-        <f>M35/$M$32</f>
+        <f>M35/$M$31</f>
         <v>0</v>
       </c>
       <c r="P35" s="40"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C36" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8">
         <v>4</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="49">
-        <v>0.89200000000000002</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="J36" s="43"/>
       <c r="K36" s="43">
-        <f t="shared" si="1"/>
-        <v>81.090909090909093</v>
+        <f>I36/$I$31</f>
+        <v>26.272727272727273</v>
       </c>
       <c r="L36" s="43"/>
       <c r="M36" s="50"/>
       <c r="N36" s="43"/>
-      <c r="O36" s="43">
-        <f>M36/$M$32</f>
-        <v>0</v>
-      </c>
+      <c r="O36" s="43"/>
       <c r="P36" s="40"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C37" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1544,22 +1537,22 @@
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="49">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="J37" s="43"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J37" s="8"/>
       <c r="K37" s="43">
-        <f>I37/$I$32</f>
-        <v>26.272727272727273</v>
-      </c>
-      <c r="L37" s="43"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
+        <f>I37/$I$31</f>
+        <v>6.6363636363636367</v>
+      </c>
+      <c r="L37" s="8"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="9"/>
       <c r="P37" s="40"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C38" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -1571,45 +1564,18 @@
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="49">
-        <v>7.2999999999999995E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="43">
-        <f>I38/$I$32</f>
-        <v>6.6363636363636367</v>
+        <f>I38/$I$31</f>
+        <v>6.0909090909090917</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="23"/>
       <c r="N38" s="8"/>
       <c r="O38" s="9"/>
       <c r="P38" s="40"/>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C39" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8">
-        <v>4</v>
-      </c>
-      <c r="G39" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="49">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="43">
-        <f>I39/$I$32</f>
-        <v>6.0909090909090917</v>
-      </c>
-      <c r="L39" s="8"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,7 +1588,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add an Error worksheet to Benchmark.xlsx to measure MSE versus passes.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Benchmarks" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="Errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Array Fill</t>
   </si>
@@ -153,6 +154,9 @@
     <t>benchmark (400, 400)</t>
   </si>
   <si>
+    <t>Passes</t>
+  </si>
+  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -169,17 +173,33 @@
   </si>
   <si>
     <t>BoxIndependentDelta</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Lucy.json</t>
+  </si>
+  <si>
+    <t>GaussianBoxDelta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +244,14 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -266,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -358,6 +386,8 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +963,7 @@
     <row r="14" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -976,7 +1006,7 @@
     <row r="16" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1008,7 +1038,7 @@
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1039,7 +1069,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1067,7 +1097,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1095,7 +1125,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1158,7 +1188,7 @@
     <row r="23" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>10</v>
@@ -1205,7 +1235,7 @@
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>10</v>
@@ -1241,7 +1271,7 @@
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>10</v>
@@ -1276,7 +1306,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>10</v>
@@ -1306,7 +1336,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>10</v>
@@ -1336,7 +1366,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>10</v>
@@ -1392,7 +1422,7 @@
     <row r="32" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32"/>
       <c r="F32" s="29">
@@ -1437,7 +1467,7 @@
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1468,7 +1498,7 @@
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1498,7 +1528,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C36" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1525,7 +1555,7 @@
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C37" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1552,7 +1582,7 @@
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C38" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -1587,9 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1616,4 +1644,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="54"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="53">
+        <v>6.3895699999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>512</v>
+      </c>
+      <c r="C8">
+        <v>1024</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="53">
+        <v>0.61456118999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="53">
+        <v>0.19017514999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="53">
+        <v>4.2626440000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="G11" s="53">
+        <v>2.0351000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="G12" s="53">
+        <v>1.6180340000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="53">
+        <v>6.7824199999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="G14" s="53">
+        <v>5.2395999999999996E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="G15" s="53">
+        <v>5.4735199999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>10000</v>
+      </c>
+      <c r="G16" s="53">
+        <v>5.4735199999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Frame the Gaussian BoxIndependentDeltaMask method. Refactor the Gaussian methods first parameter to be the result image. This is consistent with output, input order of parameters. Refactor the Gaussian calling conventions to be (row, column) consistent with m (rows) X n (columns) matrices.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Array Fill</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>GaussianBoxDelta</t>
+  </si>
+  <si>
+    <t>BoxIndependentDeltaMask</t>
   </si>
 </sst>
 </file>
@@ -716,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,146 +1155,131 @@
       <c r="P20" s="40"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I21" s="24"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-    </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="C21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
+        <v>4</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43">
+        <f>I21/$I$13</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="43"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="40"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I22" s="24"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B23" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="14">
-        <v>4</v>
-      </c>
-      <c r="I22" s="46">
+      <c r="F23" s="14">
+        <v>4</v>
+      </c>
+      <c r="I23" s="46">
         <f>0.025/4</f>
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="K22" s="15"/>
-      <c r="M22" s="28">
+      <c r="K23" s="15"/>
+      <c r="M23" s="28">
         <v>0</v>
       </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="35"/>
-    </row>
-    <row r="23" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" t="s">
+      <c r="O23" s="15"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="35"/>
+    </row>
+    <row r="24" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="19"/>
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23"/>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>23</v>
-      </c>
-      <c r="H23"/>
-      <c r="I23" s="47">
+      <c r="D24" s="34"/>
+      <c r="E24"/>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24" s="47">
         <f>19.617/4</f>
         <v>4.9042500000000002</v>
       </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11">
-        <f>I23/$I$22</f>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11">
+        <f>I24/$I$23</f>
         <v>784.68</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="24">
+      <c r="L24" s="11"/>
+      <c r="M24" s="24">
         <v>0</v>
       </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11">
-        <f>M23/$M$13</f>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11">
+        <f>M24/$M$13</f>
         <v>0</v>
       </c>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="35"/>
-    </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="35"/>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
-      <c r="C25" s="8" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8">
-        <v>4</v>
-      </c>
-      <c r="G25" s="8">
-        <v>23</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="49">
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8">
+        <v>4</v>
+      </c>
+      <c r="G26" s="8">
+        <v>23</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="49">
         <f>25.726/4</f>
         <v>6.4314999999999998</v>
       </c>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43">
-        <f>I25/$I$22</f>
-        <v>1029.04</v>
-      </c>
-      <c r="L25" s="43"/>
-      <c r="M25" s="50">
-        <v>0</v>
-      </c>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43">
-        <f>M25/$M$13</f>
-        <v>0</v>
-      </c>
-      <c r="P25" s="40"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8">
-        <v>4</v>
-      </c>
-      <c r="G26" s="8">
-        <v>23</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="49">
-        <f>2.005/4</f>
-        <v>0.50124999999999997</v>
-      </c>
       <c r="J26" s="43"/>
       <c r="K26" s="43">
-        <f>I26/$I$22</f>
-        <v>80.199999999999989</v>
+        <f>I26/$I$23</f>
+        <v>1029.04</v>
       </c>
       <c r="L26" s="43"/>
       <c r="M26" s="50">
@@ -1305,58 +1293,60 @@
       <c r="P26" s="40"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
       <c r="C27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8">
         <v>4</v>
       </c>
-      <c r="G27" s="44" t="s">
+      <c r="G27" s="8">
         <v>23</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="49">
+        <f>2.005/4</f>
+        <v>0.50124999999999997</v>
+      </c>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43">
+        <f>I27/$I$23</f>
+        <v>80.199999999999989</v>
+      </c>
+      <c r="L27" s="43"/>
+      <c r="M27" s="50">
+        <v>0</v>
+      </c>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43">
+        <f>M27/$M$13</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="40"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8">
+        <v>4</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="49">
         <f>0.731/4</f>
         <v>0.18275</v>
       </c>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43">
-        <f>I27/$I$22</f>
-        <v>29.24</v>
-      </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="40"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8">
-        <v>4</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="49">
-        <f>0.164/4</f>
-        <v>4.1000000000000002E-2</v>
-      </c>
       <c r="J28" s="43"/>
       <c r="K28" s="43">
-        <f>I28/$I$22</f>
-        <v>6.56</v>
+        <f>I28/$I$23</f>
+        <v>29.24</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="50"/>
@@ -1366,11 +1356,9 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8">
         <v>4</v>
@@ -1380,13 +1368,13 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="49">
-        <f>0.114/4</f>
-        <v>2.8500000000000001E-2</v>
+        <f>0.164/4</f>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J29" s="43"/>
       <c r="K29" s="43">
-        <f>I29/$I$22</f>
-        <v>4.5599999999999996</v>
+        <f>I29/$I$23</f>
+        <v>6.56</v>
       </c>
       <c r="L29" s="43"/>
       <c r="M29" s="50"/>
@@ -1395,194 +1383,193 @@
       <c r="P29" s="40"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I30" s="24"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-    </row>
-    <row r="31" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
+      <c r="C30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8">
+        <v>4</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="49">
+        <f>0.114/4</f>
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43">
+        <f>I30/$I$23</f>
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="40"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8">
+        <v>4</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43">
+        <f>I31/$I$23</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="43"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="40"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I32" s="24"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+    </row>
+    <row r="33" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="51">
+      <c r="I33" s="51">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="M31" s="32">
+      <c r="M33" s="32">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="35"/>
-    </row>
-    <row r="32" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" t="s">
+      <c r="P33" s="39"/>
+      <c r="Q33" s="35"/>
+    </row>
+    <row r="34" spans="2:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="19"/>
+      <c r="C34" t="s">
         <v>27</v>
       </c>
-      <c r="E32"/>
-      <c r="F32" s="29">
-        <v>4</v>
-      </c>
-      <c r="G32" s="19">
-        <v>23</v>
-      </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="47">
+      <c r="E34"/>
+      <c r="F34" s="29">
+        <v>4</v>
+      </c>
+      <c r="G34" s="19">
+        <v>23</v>
+      </c>
+      <c r="H34" s="19"/>
+      <c r="I34" s="47">
         <v>8.1280000000000001</v>
       </c>
-      <c r="J32" s="31"/>
-      <c r="K32" s="11">
-        <f t="shared" ref="K32:K35" si="1">I32/$I$31</f>
+      <c r="J34" s="31"/>
+      <c r="K34" s="11">
+        <f t="shared" ref="K34:K37" si="1">I34/$I$33</f>
         <v>738.90909090909099</v>
       </c>
-      <c r="L32" s="31"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31">
-        <f>M32/$M$31</f>
+      <c r="L34" s="31"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31">
+        <f>M34/$M$33</f>
         <v>0</v>
       </c>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="35"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="D33" s="14"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8" t="s">
+      <c r="P34" s="38"/>
+      <c r="Q34" s="35"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="D35" s="14"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+      <c r="C36" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8">
-        <v>4</v>
-      </c>
-      <c r="G34" s="8">
-        <v>23</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="49">
-        <v>10.641</v>
-      </c>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43">
-        <f t="shared" si="1"/>
-        <v>967.36363636363637</v>
-      </c>
-      <c r="L34" s="43"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43">
-        <f>M34/$M$31</f>
-        <v>0</v>
-      </c>
-      <c r="P34" s="40"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8">
-        <v>4</v>
-      </c>
-      <c r="G35" s="8">
-        <v>23</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="49">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43">
-        <f t="shared" si="1"/>
-        <v>81.090909090909093</v>
-      </c>
-      <c r="L35" s="43"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43">
-        <f>M35/$M$31</f>
-        <v>0</v>
-      </c>
-      <c r="P35" s="40"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8">
         <v>4</v>
       </c>
-      <c r="G36" s="44" t="s">
+      <c r="G36" s="8">
         <v>23</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="49">
-        <v>0.28899999999999998</v>
+        <v>10.641</v>
       </c>
       <c r="J36" s="43"/>
       <c r="K36" s="43">
-        <f>I36/$I$31</f>
-        <v>26.272727272727273</v>
+        <f t="shared" si="1"/>
+        <v>967.36363636363637</v>
       </c>
       <c r="L36" s="43"/>
       <c r="M36" s="50"/>
       <c r="N36" s="43"/>
-      <c r="O36" s="43"/>
+      <c r="O36" s="43">
+        <f>M36/$M$33</f>
+        <v>0</v>
+      </c>
       <c r="P36" s="40"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8">
         <v>4</v>
       </c>
-      <c r="G37" s="44" t="s">
+      <c r="G37" s="8">
         <v>23</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="49">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="J37" s="8"/>
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="J37" s="43"/>
       <c r="K37" s="43">
-        <f>I37/$I$31</f>
-        <v>6.6363636363636367</v>
-      </c>
-      <c r="L37" s="8"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="9"/>
+        <f t="shared" si="1"/>
+        <v>81.090909090909093</v>
+      </c>
+      <c r="L37" s="43"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43">
+        <f>M37/$M$33</f>
+        <v>0</v>
+      </c>
       <c r="P37" s="40"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C38" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -1594,18 +1581,97 @@
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="49">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43">
+        <f>I38/$I$33</f>
+        <v>26.272727272727273</v>
+      </c>
+      <c r="L38" s="43"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="40"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8">
+        <v>4</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="49">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J39" s="8"/>
+      <c r="K39" s="43">
+        <f>I39/$I$33</f>
+        <v>6.6363636363636367</v>
+      </c>
+      <c r="L39" s="8"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="40"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8">
+        <v>4</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="49">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="43">
-        <f>I38/$I$31</f>
+      <c r="J40" s="8"/>
+      <c r="K40" s="43">
+        <f>I40/$I$33</f>
         <v>6.0909090909090917</v>
       </c>
-      <c r="L38" s="8"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="40"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="40"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8">
+        <v>4</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="43">
+        <f>I41/$I$33</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="8"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete implementation of BoxIndependentMask that performs a gaussian filter with the composite mask.
</commit_message>
<xml_diff>
--- a/Relief/tests/python/Benchmark.xlsx
+++ b/Relief/tests/python/Benchmark.xlsx
@@ -190,7 +190,7 @@
     <t>GaussianBoxDelta</t>
   </si>
   <si>
-    <t>BoxIndependentDeltaMask</t>
+    <t>BoxIndependentMask</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,11 +1167,13 @@
         <v>23</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="52"/>
+      <c r="I21" s="52">
+        <v>1.714</v>
+      </c>
       <c r="J21" s="43"/>
       <c r="K21" s="43">
         <f>I21/$I$13</f>
-        <v>0</v>
+        <v>5.9103448275862069</v>
       </c>
       <c r="L21" s="43"/>
       <c r="M21" s="50"/>
@@ -1423,11 +1425,14 @@
         <v>23</v>
       </c>
       <c r="H31" s="8"/>
-      <c r="I31" s="49"/>
+      <c r="I31" s="49">
+        <f>0.251/4</f>
+        <v>6.275E-2</v>
+      </c>
       <c r="J31" s="43"/>
       <c r="K31" s="43">
         <f>I31/$I$23</f>
-        <v>0</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="L31" s="43"/>
       <c r="M31" s="50"/>

</xml_diff>